<commit_message>
Adding a comment to tun-time-stats file
</commit_message>
<xml_diff>
--- a/run-time-stats.xlsx
+++ b/run-time-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\node\calendar-model-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED06E84-F710-4385-A528-69E9EB5F54B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A9E03-2D2A-42CE-AB20-79B8BB4CE5AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4A19BDF8-CC8E-4C0D-BB5D-E70953787264}"/>
   </bookViews>
@@ -35,11 +35,20 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={108CFF23-020D-4306-990D-E33A323423D3}</author>
     <author>tc={0B500930-56FB-442E-AC9F-00CA2BCE1C74}</author>
     <author>tc={B025C206-887E-4D31-A848-27316BA63B7C}</author>
   </authors>
   <commentList>
-    <comment ref="R9" authorId="0" shapeId="0" xr:uid="{0B500930-56FB-442E-AC9F-00CA2BCE1C74}">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{108CFF23-020D-4306-990D-E33A323423D3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Non thrashing horizon</t>
+      </text>
+    </comment>
+    <comment ref="R9" authorId="1" shapeId="0" xr:uid="{0B500930-56FB-442E-AC9F-00CA2BCE1C74}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +56,7 @@
     Point of highest difference.</t>
       </text>
     </comment>
-    <comment ref="R13" authorId="1" shapeId="0" xr:uid="{B025C206-887E-4D31-A848-27316BA63B7C}">
+    <comment ref="R13" authorId="2" shapeId="0" xr:uid="{B025C206-887E-4D31-A848-27316BA63B7C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -93,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,8 +147,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +172,11 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
       </patternFill>
     </fill>
   </fills>
@@ -205,12 +226,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,10 +249,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="Accent4" xfId="3" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4778,6 +4802,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="R5" dT="2020-07-01T14:14:34.31" personId="{8FC7673D-FF73-4B7A-9BC4-48642237F644}" id="{108CFF23-020D-4306-990D-E33A323423D3}">
+    <text>Non thrashing horizon</text>
+  </threadedComment>
   <threadedComment ref="R9" dT="2020-07-01T13:42:39.82" personId="{8FC7673D-FF73-4B7A-9BC4-48642237F644}" id="{0B500930-56FB-442E-AC9F-00CA2BCE1C74}">
     <text>Point of highest difference.</text>
   </threadedComment>
@@ -4855,7 +4882,7 @@
         <v>101</v>
       </c>
       <c r="I3">
-        <f>((D3-G3)/H3)</f>
+        <f t="shared" ref="I3:I21" si="0">((D3-G3)/H3)</f>
         <v>0.99009900990099009</v>
       </c>
     </row>
@@ -4882,7 +4909,7 @@
         <v>121</v>
       </c>
       <c r="I4">
-        <f>((D4-G4)/H4)</f>
+        <f t="shared" si="0"/>
         <v>1.1487603305785123</v>
       </c>
     </row>
@@ -4909,7 +4936,7 @@
         <v>121</v>
       </c>
       <c r="I5">
-        <f>((D5-G5)/H5)</f>
+        <f t="shared" si="0"/>
         <v>1.3471074380165289</v>
       </c>
     </row>
@@ -4936,7 +4963,7 @@
         <v>121</v>
       </c>
       <c r="I6">
-        <f>((D6-G6)/H6)</f>
+        <f t="shared" si="0"/>
         <v>1.5619834710743801</v>
       </c>
     </row>
@@ -4963,7 +4990,7 @@
         <v>121</v>
       </c>
       <c r="I7">
-        <f>((D7-G7)/H7)</f>
+        <f t="shared" si="0"/>
         <v>1.5289256198347108</v>
       </c>
     </row>
@@ -4990,7 +5017,7 @@
         <v>121</v>
       </c>
       <c r="I8">
-        <f>((D8-G8)/H8)</f>
+        <f t="shared" si="0"/>
         <v>1.6446280991735538</v>
       </c>
     </row>
@@ -5017,7 +5044,7 @@
         <v>121</v>
       </c>
       <c r="I9">
-        <f>((D9-G9)/H9)</f>
+        <f t="shared" si="0"/>
         <v>2.0413223140495869</v>
       </c>
     </row>
@@ -5044,7 +5071,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <f>((D10-G10)/H10)</f>
+        <f t="shared" si="0"/>
         <v>1.9256198347107438</v>
       </c>
     </row>
@@ -5071,7 +5098,7 @@
         <v>122</v>
       </c>
       <c r="I11">
-        <f>((D11-G11)/H11)</f>
+        <f t="shared" si="0"/>
         <v>2.3114754098360657</v>
       </c>
     </row>
@@ -5098,7 +5125,7 @@
         <v>122</v>
       </c>
       <c r="I12">
-        <f>((D12-G12)/H12)</f>
+        <f t="shared" si="0"/>
         <v>2.459016393442623</v>
       </c>
     </row>
@@ -5125,7 +5152,7 @@
         <v>122</v>
       </c>
       <c r="I13">
-        <f>((D13-G13)/H13)</f>
+        <f t="shared" si="0"/>
         <v>2.7704918032786887</v>
       </c>
     </row>
@@ -5152,7 +5179,7 @@
         <v>122</v>
       </c>
       <c r="I14">
-        <f>((D14-G14)/H14)</f>
+        <f t="shared" si="0"/>
         <v>3.098360655737705</v>
       </c>
     </row>
@@ -5179,7 +5206,7 @@
         <v>122</v>
       </c>
       <c r="I15">
-        <f>((D15-G15)/H15)</f>
+        <f t="shared" si="0"/>
         <v>3.081967213114754</v>
       </c>
     </row>
@@ -5206,7 +5233,7 @@
         <v>122</v>
       </c>
       <c r="I16">
-        <f>((D16-G16)/H16)</f>
+        <f t="shared" si="0"/>
         <v>3.377049180327869</v>
       </c>
     </row>
@@ -5233,7 +5260,7 @@
         <v>122</v>
       </c>
       <c r="I17">
-        <f>((D17-G17)/H17)</f>
+        <f t="shared" si="0"/>
         <v>3.6065573770491803</v>
       </c>
     </row>
@@ -5260,7 +5287,7 @@
         <v>122</v>
       </c>
       <c r="I18">
-        <f>((D18-G18)/H18)</f>
+        <f t="shared" si="0"/>
         <v>3.7131147540983607</v>
       </c>
     </row>
@@ -5287,7 +5314,7 @@
         <v>122</v>
       </c>
       <c r="I19">
-        <f>((D19-G19)/H19)</f>
+        <f t="shared" si="0"/>
         <v>3.877049180327869</v>
       </c>
     </row>
@@ -5314,7 +5341,7 @@
         <v>122</v>
       </c>
       <c r="I20">
-        <f>((D20-G20)/H20)</f>
+        <f t="shared" si="0"/>
         <v>4.3770491803278686</v>
       </c>
     </row>
@@ -5341,7 +5368,7 @@
         <v>122</v>
       </c>
       <c r="I21">
-        <f>((D21-G21)/H21)</f>
+        <f t="shared" si="0"/>
         <v>4.581967213114754</v>
       </c>
     </row>
@@ -5420,7 +5447,7 @@
         <v>41</v>
       </c>
       <c r="I3">
-        <f>((D3-G3)/H3)</f>
+        <f t="shared" ref="I3:I21" si="0">((D3-G3)/H3)</f>
         <v>2.4390243902439024</v>
       </c>
     </row>
@@ -5447,7 +5474,7 @@
         <v>68</v>
       </c>
       <c r="I4">
-        <f>((D4-G4)/H4)</f>
+        <f t="shared" si="0"/>
         <v>2.2058823529411766</v>
       </c>
     </row>
@@ -5474,7 +5501,7 @@
         <v>83</v>
       </c>
       <c r="I5">
-        <f>((D5-G5)/H5)</f>
+        <f t="shared" si="0"/>
         <v>2.4096385542168677</v>
       </c>
     </row>
@@ -5501,7 +5528,7 @@
         <v>100</v>
       </c>
       <c r="I6">
-        <f>((D6-G6)/H6)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -5528,7 +5555,7 @@
         <v>121</v>
       </c>
       <c r="I7">
-        <f>((D7-G7)/H7)</f>
+        <f t="shared" si="0"/>
         <v>2.2892561983471076</v>
       </c>
     </row>
@@ -5555,7 +5582,7 @@
         <v>121</v>
       </c>
       <c r="I8">
-        <f>((D8-G8)/H8)</f>
+        <f t="shared" si="0"/>
         <v>2.4958677685950414</v>
       </c>
     </row>
@@ -5582,7 +5609,7 @@
         <v>121</v>
       </c>
       <c r="I9">
-        <f>((D9-G9)/H9)</f>
+        <f t="shared" si="0"/>
         <v>2.8925619834710745</v>
       </c>
     </row>
@@ -5609,7 +5636,7 @@
         <v>121</v>
       </c>
       <c r="I10">
-        <f>((D10-G10)/H10)</f>
+        <f t="shared" si="0"/>
         <v>3.1239669421487601</v>
       </c>
     </row>
@@ -5636,7 +5663,7 @@
         <v>122</v>
       </c>
       <c r="I11">
-        <f>((D11-G11)/H11)</f>
+        <f t="shared" si="0"/>
         <v>3.2295081967213113</v>
       </c>
     </row>
@@ -5663,7 +5690,7 @@
         <v>122</v>
       </c>
       <c r="I12">
-        <f>((D12-G12)/H12)</f>
+        <f t="shared" si="0"/>
         <v>2.8442622950819674</v>
       </c>
     </row>
@@ -5690,7 +5717,7 @@
         <v>122</v>
       </c>
       <c r="I13">
-        <f>((D13-G13)/H13)</f>
+        <f t="shared" si="0"/>
         <v>2.8032786885245899</v>
       </c>
     </row>
@@ -5717,7 +5744,7 @@
         <v>122</v>
       </c>
       <c r="I14">
-        <f>((D14-G14)/H14)</f>
+        <f t="shared" si="0"/>
         <v>2.9262295081967213</v>
       </c>
     </row>
@@ -5744,7 +5771,7 @@
         <v>122</v>
       </c>
       <c r="I15">
-        <f>((D15-G15)/H15)</f>
+        <f t="shared" si="0"/>
         <v>3.1557377049180326</v>
       </c>
     </row>
@@ -5771,7 +5798,7 @@
         <v>122</v>
       </c>
       <c r="I16">
-        <f>((D16-G16)/H16)</f>
+        <f t="shared" si="0"/>
         <v>3.2459016393442623</v>
       </c>
     </row>
@@ -5798,7 +5825,7 @@
         <v>122</v>
       </c>
       <c r="I17">
-        <f>((D17-G17)/H17)</f>
+        <f t="shared" si="0"/>
         <v>3.737704918032787</v>
       </c>
     </row>
@@ -5825,7 +5852,7 @@
         <v>122</v>
       </c>
       <c r="I18">
-        <f>((D18-G18)/H18)</f>
+        <f t="shared" si="0"/>
         <v>3.7868852459016393</v>
       </c>
     </row>
@@ -5852,7 +5879,7 @@
         <v>122</v>
       </c>
       <c r="I19">
-        <f>((D19-G19)/H19)</f>
+        <f t="shared" si="0"/>
         <v>4.3524590163934427</v>
       </c>
     </row>
@@ -5879,7 +5906,7 @@
         <v>122</v>
       </c>
       <c r="I20">
-        <f>((D20-G20)/H20)</f>
+        <f t="shared" si="0"/>
         <v>4.1147540983606561</v>
       </c>
     </row>
@@ -5906,7 +5933,7 @@
         <v>122</v>
       </c>
       <c r="I21">
-        <f>((D21-G21)/H21)</f>
+        <f t="shared" si="0"/>
         <v>4.3852459016393439</v>
       </c>
     </row>
@@ -5922,7 +5949,7 @@
   <dimension ref="B1:T20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6008,7 +6035,7 @@
         <v>101</v>
       </c>
       <c r="I2">
-        <f>((D2-G2)/H2)</f>
+        <f t="shared" ref="I2:I20" si="0">((D2-G2)/H2)</f>
         <v>0.99009900990099009</v>
       </c>
       <c r="K2">
@@ -6033,11 +6060,11 @@
         <v>41</v>
       </c>
       <c r="R2">
-        <f>((M2-P2)/Q2)</f>
+        <f t="shared" ref="R2:R20" si="1">((M2-P2)/Q2)</f>
         <v>2.4390243902439024</v>
       </c>
       <c r="T2" s="7">
-        <f>R2-I2</f>
+        <f t="shared" ref="T2:T20" si="2">R2-I2</f>
         <v>1.4489253803429123</v>
       </c>
     </row>
@@ -6064,7 +6091,7 @@
         <v>121</v>
       </c>
       <c r="I3">
-        <f>((D3-G3)/H3)</f>
+        <f t="shared" si="0"/>
         <v>1.1487603305785123</v>
       </c>
       <c r="K3">
@@ -6089,11 +6116,11 @@
         <v>68</v>
       </c>
       <c r="R3">
-        <f>((M3-P3)/Q3)</f>
+        <f t="shared" si="1"/>
         <v>2.2058823529411766</v>
       </c>
       <c r="T3" s="7">
-        <f>R3-I3</f>
+        <f t="shared" si="2"/>
         <v>1.0571220223626643</v>
       </c>
     </row>
@@ -6120,7 +6147,7 @@
         <v>121</v>
       </c>
       <c r="I4">
-        <f>((D4-G4)/H4)</f>
+        <f t="shared" si="0"/>
         <v>1.3471074380165289</v>
       </c>
       <c r="K4">
@@ -6145,67 +6172,68 @@
         <v>83</v>
       </c>
       <c r="R4">
-        <f>((M4-P4)/Q4)</f>
+        <f t="shared" si="1"/>
         <v>2.4096385542168677</v>
       </c>
       <c r="T4" s="7">
-        <f>R4-I4</f>
+        <f t="shared" si="2"/>
         <v>1.0625311162003388</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B5">
+      <c r="B5" s="12">
         <v>2000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>250</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="12">
         <v>189</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
         <v>61</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
         <v>121</v>
       </c>
-      <c r="I5">
-        <f>((D5-G5)/H5)</f>
+      <c r="I5" s="12">
+        <f t="shared" si="0"/>
         <v>1.5619834710743801</v>
       </c>
-      <c r="K5">
+      <c r="J5" s="12"/>
+      <c r="K5" s="12">
         <v>1000</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="12">
         <v>250</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="12">
         <v>250</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
+      <c r="N5" s="12">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="12">
         <v>100</v>
       </c>
-      <c r="R5">
-        <f>((M5-P5)/Q5)</f>
+      <c r="R5" s="12">
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
-      <c r="T5" s="7">
-        <f>R5-I5</f>
+      <c r="T5" s="12">
+        <f t="shared" si="2"/>
         <v>0.93801652892561993</v>
       </c>
     </row>
@@ -6232,7 +6260,7 @@
         <v>121</v>
       </c>
       <c r="I6">
-        <f>((D6-G6)/H6)</f>
+        <f t="shared" si="0"/>
         <v>1.5289256198347108</v>
       </c>
       <c r="K6">
@@ -6257,11 +6285,11 @@
         <v>121</v>
       </c>
       <c r="R6">
-        <f>((M6-P6)/Q6)</f>
+        <f t="shared" si="1"/>
         <v>2.2892561983471076</v>
       </c>
       <c r="T6" s="7">
-        <f>R6-I6</f>
+        <f t="shared" si="2"/>
         <v>0.76033057851239683</v>
       </c>
     </row>
@@ -6288,7 +6316,7 @@
         <v>121</v>
       </c>
       <c r="I7">
-        <f>((D7-G7)/H7)</f>
+        <f t="shared" si="0"/>
         <v>1.6446280991735538</v>
       </c>
       <c r="K7">
@@ -6313,11 +6341,11 @@
         <v>121</v>
       </c>
       <c r="R7">
-        <f>((M7-P7)/Q7)</f>
+        <f t="shared" si="1"/>
         <v>2.4958677685950414</v>
       </c>
       <c r="T7" s="7">
-        <f>R7-I7</f>
+        <f t="shared" si="2"/>
         <v>0.85123966942148765</v>
       </c>
     </row>
@@ -6344,7 +6372,7 @@
         <v>121</v>
       </c>
       <c r="I8">
-        <f>((D8-G8)/H8)</f>
+        <f t="shared" si="0"/>
         <v>2.0413223140495869</v>
       </c>
       <c r="K8">
@@ -6369,11 +6397,11 @@
         <v>121</v>
       </c>
       <c r="R8">
-        <f>((M8-P8)/Q8)</f>
+        <f t="shared" si="1"/>
         <v>2.8925619834710745</v>
       </c>
       <c r="T8" s="7">
-        <f>R8-I8</f>
+        <f t="shared" si="2"/>
         <v>0.85123966942148765</v>
       </c>
     </row>
@@ -6400,7 +6428,7 @@
         <v>121</v>
       </c>
       <c r="I9" s="6">
-        <f>((D9-G9)/H9)</f>
+        <f t="shared" si="0"/>
         <v>1.9256198347107438</v>
       </c>
       <c r="J9" s="6"/>
@@ -6426,11 +6454,11 @@
         <v>121</v>
       </c>
       <c r="R9" s="6">
-        <f>((M9-P9)/Q9)</f>
+        <f t="shared" si="1"/>
         <v>3.1239669421487601</v>
       </c>
       <c r="T9" s="8">
-        <f>R9-I9</f>
+        <f t="shared" si="2"/>
         <v>1.1983471074380163</v>
       </c>
     </row>
@@ -6457,7 +6485,7 @@
         <v>122</v>
       </c>
       <c r="I10">
-        <f>((D10-G10)/H10)</f>
+        <f t="shared" si="0"/>
         <v>2.3114754098360657</v>
       </c>
       <c r="K10">
@@ -6482,11 +6510,11 @@
         <v>122</v>
       </c>
       <c r="R10">
-        <f>((M10-P10)/Q10)</f>
+        <f t="shared" si="1"/>
         <v>3.2295081967213113</v>
       </c>
       <c r="T10" s="7">
-        <f>R10-I10</f>
+        <f t="shared" si="2"/>
         <v>0.91803278688524559</v>
       </c>
     </row>
@@ -6513,7 +6541,7 @@
         <v>122</v>
       </c>
       <c r="I11">
-        <f>((D11-G11)/H11)</f>
+        <f t="shared" si="0"/>
         <v>2.459016393442623</v>
       </c>
       <c r="K11">
@@ -6538,11 +6566,11 @@
         <v>122</v>
       </c>
       <c r="R11">
-        <f>((M11-P11)/Q11)</f>
+        <f t="shared" si="1"/>
         <v>2.8442622950819674</v>
       </c>
       <c r="T11" s="7">
-        <f>R11-I11</f>
+        <f t="shared" si="2"/>
         <v>0.38524590163934436</v>
       </c>
     </row>
@@ -6569,7 +6597,7 @@
         <v>122</v>
       </c>
       <c r="I12">
-        <f>((D12-G12)/H12)</f>
+        <f t="shared" si="0"/>
         <v>2.7704918032786887</v>
       </c>
       <c r="K12">
@@ -6594,11 +6622,11 @@
         <v>122</v>
       </c>
       <c r="R12">
-        <f>((M12-P12)/Q12)</f>
+        <f t="shared" si="1"/>
         <v>2.8032786885245899</v>
       </c>
       <c r="T12" s="7">
-        <f>R12-I12</f>
+        <f t="shared" si="2"/>
         <v>3.2786885245901232E-2</v>
       </c>
     </row>
@@ -6625,7 +6653,7 @@
         <v>122</v>
       </c>
       <c r="I13" s="3">
-        <f>((D13-G13)/H13)</f>
+        <f t="shared" si="0"/>
         <v>3.098360655737705</v>
       </c>
       <c r="J13" s="3"/>
@@ -6651,11 +6679,11 @@
         <v>122</v>
       </c>
       <c r="R13" s="3">
-        <f>((M13-P13)/Q13)</f>
+        <f t="shared" si="1"/>
         <v>2.9262295081967213</v>
       </c>
       <c r="T13" s="9">
-        <f>R13-I13</f>
+        <f t="shared" si="2"/>
         <v>-0.17213114754098369</v>
       </c>
     </row>
@@ -6682,7 +6710,7 @@
         <v>122</v>
       </c>
       <c r="I14">
-        <f>((D14-G14)/H14)</f>
+        <f t="shared" si="0"/>
         <v>3.081967213114754</v>
       </c>
       <c r="K14">
@@ -6707,11 +6735,11 @@
         <v>122</v>
       </c>
       <c r="R14">
-        <f>((M14-P14)/Q14)</f>
+        <f t="shared" si="1"/>
         <v>3.1557377049180326</v>
       </c>
       <c r="T14" s="7">
-        <f>R14-I14</f>
+        <f t="shared" si="2"/>
         <v>7.3770491803278659E-2</v>
       </c>
     </row>
@@ -6738,7 +6766,7 @@
         <v>122</v>
       </c>
       <c r="I15">
-        <f>((D15-G15)/H15)</f>
+        <f t="shared" si="0"/>
         <v>3.377049180327869</v>
       </c>
       <c r="K15">
@@ -6763,11 +6791,11 @@
         <v>122</v>
       </c>
       <c r="R15">
-        <f>((M15-P15)/Q15)</f>
+        <f t="shared" si="1"/>
         <v>3.2459016393442623</v>
       </c>
       <c r="T15" s="7">
-        <f>R15-I15</f>
+        <f t="shared" si="2"/>
         <v>-0.1311475409836067</v>
       </c>
     </row>
@@ -6794,7 +6822,7 @@
         <v>122</v>
       </c>
       <c r="I16">
-        <f>((D16-G16)/H16)</f>
+        <f t="shared" si="0"/>
         <v>3.6065573770491803</v>
       </c>
       <c r="K16">
@@ -6819,11 +6847,11 @@
         <v>122</v>
       </c>
       <c r="R16">
-        <f>((M16-P16)/Q16)</f>
+        <f t="shared" si="1"/>
         <v>3.737704918032787</v>
       </c>
       <c r="T16" s="7">
-        <f>R16-I16</f>
+        <f t="shared" si="2"/>
         <v>0.1311475409836067</v>
       </c>
     </row>
@@ -6850,7 +6878,7 @@
         <v>122</v>
       </c>
       <c r="I17">
-        <f>((D17-G17)/H17)</f>
+        <f t="shared" si="0"/>
         <v>3.7131147540983607</v>
       </c>
       <c r="K17">
@@ -6875,11 +6903,11 @@
         <v>122</v>
       </c>
       <c r="R17">
-        <f>((M17-P17)/Q17)</f>
+        <f t="shared" si="1"/>
         <v>3.7868852459016393</v>
       </c>
       <c r="T17" s="7">
-        <f>R17-I17</f>
+        <f t="shared" si="2"/>
         <v>7.3770491803278659E-2</v>
       </c>
     </row>
@@ -6906,7 +6934,7 @@
         <v>122</v>
       </c>
       <c r="I18">
-        <f>((D18-G18)/H18)</f>
+        <f t="shared" si="0"/>
         <v>3.877049180327869</v>
       </c>
       <c r="K18">
@@ -6931,11 +6959,11 @@
         <v>122</v>
       </c>
       <c r="R18">
-        <f>((M18-P18)/Q18)</f>
+        <f t="shared" si="1"/>
         <v>4.3524590163934427</v>
       </c>
       <c r="T18" s="7">
-        <f>R18-I18</f>
+        <f t="shared" si="2"/>
         <v>0.47540983606557363</v>
       </c>
     </row>
@@ -6962,7 +6990,7 @@
         <v>122</v>
       </c>
       <c r="I19">
-        <f>((D19-G19)/H19)</f>
+        <f t="shared" si="0"/>
         <v>4.3770491803278686</v>
       </c>
       <c r="K19">
@@ -6987,11 +7015,11 @@
         <v>122</v>
       </c>
       <c r="R19">
-        <f>((M19-P19)/Q19)</f>
+        <f t="shared" si="1"/>
         <v>4.1147540983606561</v>
       </c>
       <c r="T19" s="7">
-        <f>R19-I19</f>
+        <f t="shared" si="2"/>
         <v>-0.26229508196721252</v>
       </c>
     </row>
@@ -7018,7 +7046,7 @@
         <v>122</v>
       </c>
       <c r="I20">
-        <f>((D20-G20)/H20)</f>
+        <f t="shared" si="0"/>
         <v>4.581967213114754</v>
       </c>
       <c r="K20">
@@ -7043,11 +7071,11 @@
         <v>122</v>
       </c>
       <c r="R20">
-        <f>((M20-P20)/Q20)</f>
+        <f t="shared" si="1"/>
         <v>4.3852459016393439</v>
       </c>
       <c r="T20" s="10">
-        <f>R20-I20</f>
+        <f t="shared" si="2"/>
         <v>-0.19672131147541005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Committing new delegate queue implementation using async.queue
</commit_message>
<xml_diff>
--- a/run-time-stats.xlsx
+++ b/run-time-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\node\calendar-model-setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A9E03-2D2A-42CE-AB20-79B8BB4CE5AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B4332E-6786-479A-AFE6-405BD9266D0F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{4A19BDF8-CC8E-4C0D-BB5D-E70953787264}"/>
   </bookViews>
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,12 +140,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -230,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -249,7 +243,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -5948,8 +5942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9E98F4-F532-47BB-B9E8-46185575FB2B}">
   <dimension ref="B1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6035,7 +6029,7 @@
         <v>101</v>
       </c>
       <c r="I2">
-        <f t="shared" ref="I2:I20" si="0">((D2-G2)/H2)</f>
+        <f t="shared" ref="I2:I19" si="0">((D2-G2)/H2)</f>
         <v>0.99009900990099009</v>
       </c>
       <c r="K2">
@@ -7046,7 +7040,7 @@
         <v>122</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f>((D20-G20)/H20)</f>
         <v>4.581967213114754</v>
       </c>
       <c r="K20">

</xml_diff>